<commit_message>
finishe dfirst round reviewer edits
</commit_message>
<xml_diff>
--- a/data_submission/mag_details.xlsx
+++ b/data_submission/mag_details.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guritsk1/Desktop/timeline_paper/figures_and_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guritsk1/Desktop/timeline_paper/data_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="460" windowWidth="24520" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="4280" yWindow="460" windowWidth="29660" windowHeight="25000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -981,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="93" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2117,7 +2117,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>160</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -2327,497 +2327,539 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="2">
         <v>91.15</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <v>0.8</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
         <v>0.65100000000000002</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="2">
         <v>16850</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <v>2603423</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="2">
         <v>216</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="2">
         <v>25.537099999999999</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="2">
         <v>0.18138352428999999</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K39" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <v>90.29</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <v>2</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
         <v>0.64500000000000002</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="2">
         <v>6411</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <v>2721633</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="2">
         <v>511</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="2">
         <v>25.999300000000002</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="2">
         <v>0.204788098157</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="K40" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>74.92</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>1.615</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>0.65200000000000002</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>4719</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>2069396</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>480</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="2">
         <v>6.5011400000000004</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="2">
         <v>9.6169606250399997E-2</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>75.099999999999994</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>1.5329999999999999</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>0.65800000000000003</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>3129</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>1918756</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>665</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="2">
         <v>15.9353</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="2">
         <v>2.44123282253</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>82.18</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="2">
         <v>2.5529999999999999</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>0.66200000000000003</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>3574</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>2099664</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>658</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="2">
         <v>5.4398900000000001</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="2">
         <v>0.85196636327499997</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K43" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>72.47</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="2">
         <v>1.8</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>0.65700000000000003</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>3389</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="2">
         <v>2173558</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>739</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="2">
         <v>56.4711</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="2">
         <v>3.2386193518900002</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>72.989999999999995</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>1.2330000000000001</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>0.66300000000000003</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>5746</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="2">
         <v>1892619</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>390</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="2">
         <v>7.2593699999999997</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="2">
         <v>8.2451564577200003</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K45" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="2">
         <v>94.84</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <v>2.8149999999999999</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
         <v>0.66600000000000004</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="2">
         <v>12192</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="2">
         <v>3181126</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="2">
         <v>354</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="2">
         <v>9.5159300000000009</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="2">
         <v>2.2001650971900002</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K46" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>74.23</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <v>2</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="2">
         <v>0.67100000000000004</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="2">
         <v>4858</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="2">
         <v>2284265</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="2">
         <v>602</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="2">
         <v>9.5233399999999993</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="2">
         <v>2.7439343193600001</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K47" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>78.790000000000006</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>0.67300000000000004</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>3724</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="2">
         <v>1469027</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="2">
         <v>471</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="2">
         <v>13.3886</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="2">
         <v>2.84170697306</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K48" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>73.94</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="2">
         <v>2.0209999999999999</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>0.67</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>2547</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>1954103</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2">
         <v>787</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="2">
         <v>221.91200000000001</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="2">
         <v>0.16151653510200001</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K49" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="2">
         <v>72.180000000000007</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>1.0629999999999999</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>0.66800000000000004</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>8025</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>1841689</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>310</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="2">
         <v>5.4245700000000001</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="2">
         <v>1.82360146632</v>
       </c>
-      <c r="K50" t="s">
+      <c r="K50" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>86.13</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>1.4</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>7135</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2">
         <v>2514956</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <v>453</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="2">
         <v>10.4039</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="2">
         <v>0.24911757512499999</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K51" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="2">
         <v>74.03</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>1.2</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>0.68200000000000005</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>3137</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="2">
         <v>2161520</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <v>755</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="2">
         <v>14.885199999999999</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="2">
         <v>1.9849744756100001</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K52" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2852,7 +2894,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -2887,7 +2929,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -2922,7 +2964,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -2957,7 +2999,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>165</v>
       </c>
@@ -2992,7 +3034,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>155</v>
       </c>
@@ -3027,7 +3069,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3062,7 +3104,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>169</v>
       </c>
@@ -3097,7 +3139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -3132,7 +3174,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -3167,7 +3209,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -3202,7 +3244,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>168</v>
       </c>

</xml_diff>